<commit_message>
Made lat and long into range columns
</commit_message>
<xml_diff>
--- a/Raw_data/location_data_full.xlsx
+++ b/Raw_data/location_data_full.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bop22abs/Documents/PhD/Chapter_1_code/Raw_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bop22abs/Documents/PhD/Chapter_1_code/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EC12EB2-C94D-4E46-9194-4449E1F1EC21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFD2E769-D996-CA4C-BC20-21E1AA497DCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38000" yWindow="-7900" windowWidth="34380" windowHeight="26460" xr2:uid="{7DB4B7B0-8D04-9C4D-8F34-A11A49669C1B}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" xr2:uid="{7DB4B7B0-8D04-9C4D-8F34-A11A49669C1B}"/>
   </bookViews>
   <sheets>
     <sheet name="location_raw" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">location_raw!$A$1:$I$771</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">location_raw!$A$1:$I$777</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5872" uniqueCount="2615">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5928" uniqueCount="2635">
   <si>
     <t>location.code</t>
   </si>
@@ -7884,6 +7884,66 @@
   </si>
   <si>
     <t>18.423149</t>
+  </si>
+  <si>
+    <t>Colombia</t>
+  </si>
+  <si>
+    <t>loc-794</t>
+  </si>
+  <si>
+    <t>loc-795</t>
+  </si>
+  <si>
+    <t>loc-796</t>
+  </si>
+  <si>
+    <t>loc-797</t>
+  </si>
+  <si>
+    <t>loc-798</t>
+  </si>
+  <si>
+    <t>-38.416105</t>
+  </si>
+  <si>
+    <t>-63.616671</t>
+  </si>
+  <si>
+    <t>-14.234998</t>
+  </si>
+  <si>
+    <t>-51.925281</t>
+  </si>
+  <si>
+    <t>-32.522772</t>
+  </si>
+  <si>
+    <t>-55.765840</t>
+  </si>
+  <si>
+    <t>4.570863</t>
+  </si>
+  <si>
+    <t>-74.297329</t>
+  </si>
+  <si>
+    <t>50.579996</t>
+  </si>
+  <si>
+    <t>13.000000</t>
+  </si>
+  <si>
+    <t>55.755703</t>
+  </si>
+  <si>
+    <t>37.617384</t>
+  </si>
+  <si>
+    <t>12.666042</t>
+  </si>
+  <si>
+    <t>31.659416</t>
   </si>
 </sst>
 </file>
@@ -8365,11 +8425,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CF586FE-D329-5147-97C1-F707C19E06F5}">
-  <dimension ref="A1:I771"/>
+  <dimension ref="A1:I777"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E773" sqref="E773"/>
+      <pane ySplit="1" topLeftCell="A748" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H769" sqref="H769"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -27325,6 +27385,12 @@
       <c r="G667" s="5" t="s">
         <v>13</v>
       </c>
+      <c r="H667" s="6" t="s">
+        <v>2629</v>
+      </c>
+      <c r="I667" s="6" t="s">
+        <v>2630</v>
+      </c>
     </row>
     <row r="668" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A668" s="5" t="s">
@@ -29288,6 +29354,12 @@
       <c r="G735" s="5" t="s">
         <v>13</v>
       </c>
+      <c r="H735" s="6" t="s">
+        <v>2631</v>
+      </c>
+      <c r="I735" s="6" t="s">
+        <v>2632</v>
+      </c>
     </row>
     <row r="736" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A736" s="5" t="s">
@@ -29418,6 +29490,12 @@
       <c r="G740" s="5" t="s">
         <v>13</v>
       </c>
+      <c r="H740" s="6" t="s">
+        <v>2631</v>
+      </c>
+      <c r="I740" s="6" t="s">
+        <v>2632</v>
+      </c>
     </row>
     <row r="741" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A741" s="5" t="s">
@@ -29640,6 +29718,12 @@
       </c>
       <c r="G748" s="5" t="s">
         <v>530</v>
+      </c>
+      <c r="H748" s="6" t="s">
+        <v>2633</v>
+      </c>
+      <c r="I748" s="6" t="s">
+        <v>2634</v>
       </c>
     </row>
     <row r="749" spans="1:9" x14ac:dyDescent="0.2">
@@ -30254,8 +30338,182 @@
         <v>2565</v>
       </c>
     </row>
+    <row r="772" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A772" s="5" t="s">
+        <v>2216</v>
+      </c>
+      <c r="B772" s="5">
+        <v>1313</v>
+      </c>
+      <c r="C772" s="5" t="s">
+        <v>584</v>
+      </c>
+      <c r="D772" s="5" t="s">
+        <v>864</v>
+      </c>
+      <c r="E772" s="5" t="s">
+        <v>584</v>
+      </c>
+      <c r="F772" s="5" t="s">
+        <v>584</v>
+      </c>
+      <c r="G772" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H772" s="6" t="s">
+        <v>2591</v>
+      </c>
+      <c r="I772" s="6" t="s">
+        <v>2592</v>
+      </c>
+    </row>
+    <row r="773" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A773" s="5" t="s">
+        <v>2616</v>
+      </c>
+      <c r="B773" s="5">
+        <v>1313</v>
+      </c>
+      <c r="C773" s="5" t="s">
+        <v>389</v>
+      </c>
+      <c r="D773" s="5" t="s">
+        <v>864</v>
+      </c>
+      <c r="E773" s="5" t="s">
+        <v>389</v>
+      </c>
+      <c r="F773" s="5" t="s">
+        <v>389</v>
+      </c>
+      <c r="G773" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="H773" s="6" t="s">
+        <v>2621</v>
+      </c>
+      <c r="I773" s="6" t="s">
+        <v>2622</v>
+      </c>
+    </row>
+    <row r="774" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A774" s="5" t="s">
+        <v>2617</v>
+      </c>
+      <c r="B774" s="5">
+        <v>1313</v>
+      </c>
+      <c r="C774" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="D774" s="5" t="s">
+        <v>864</v>
+      </c>
+      <c r="E774" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="F774" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="G774" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="H774" s="6" t="s">
+        <v>2623</v>
+      </c>
+      <c r="I774" s="6" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="775" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A775" s="5" t="s">
+        <v>2618</v>
+      </c>
+      <c r="B775" s="5">
+        <v>1313</v>
+      </c>
+      <c r="C775" s="5" t="s">
+        <v>385</v>
+      </c>
+      <c r="D775" s="5" t="s">
+        <v>864</v>
+      </c>
+      <c r="E775" s="5" t="s">
+        <v>385</v>
+      </c>
+      <c r="F775" s="5" t="s">
+        <v>385</v>
+      </c>
+      <c r="G775" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="H775" s="6" t="s">
+        <v>2625</v>
+      </c>
+      <c r="I775" s="6" t="s">
+        <v>2626</v>
+      </c>
+    </row>
+    <row r="776" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A776" s="5" t="s">
+        <v>2619</v>
+      </c>
+      <c r="B776" s="5">
+        <v>1313</v>
+      </c>
+      <c r="C776" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D776" s="5" t="s">
+        <v>864</v>
+      </c>
+      <c r="E776" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="F776" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="G776" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="H776" s="6" t="s">
+        <v>2605</v>
+      </c>
+      <c r="I776" s="6" t="s">
+        <v>2606</v>
+      </c>
+    </row>
+    <row r="777" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A777" s="5" t="s">
+        <v>2620</v>
+      </c>
+      <c r="B777" s="5">
+        <v>1313</v>
+      </c>
+      <c r="C777" s="5" t="s">
+        <v>2615</v>
+      </c>
+      <c r="D777" s="5" t="s">
+        <v>864</v>
+      </c>
+      <c r="E777" s="5" t="s">
+        <v>2615</v>
+      </c>
+      <c r="F777" s="5" t="s">
+        <v>2615</v>
+      </c>
+      <c r="G777" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="H777" s="6" t="s">
+        <v>2627</v>
+      </c>
+      <c r="I777" s="6" t="s">
+        <v>2628</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:I771" xr:uid="{3CF586FE-D329-5147-97C1-F707C19E06F5}"/>
+  <autoFilter ref="A1:I777" xr:uid="{3CF586FE-D329-5147-97C1-F707C19E06F5}"/>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Re ran all scripts and just need to do final body sizew script and then completed database
</commit_message>
<xml_diff>
--- a/Raw_data/location_data_full.xlsx
+++ b/Raw_data/location_data_full.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bop22abs/Documents/PhD/Chapter_1_code/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFD2E769-D996-CA4C-BC20-21E1AA497DCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDFFBD1E-FADB-3342-AC41-10306BF64B18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" xr2:uid="{7DB4B7B0-8D04-9C4D-8F34-A11A49669C1B}"/>
   </bookViews>
@@ -8428,8 +8428,8 @@
   <dimension ref="A1:I777"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A748" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H769" sqref="H769"/>
+      <pane ySplit="1" topLeftCell="A335" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F344" sqref="F344"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
sorting out final edits
</commit_message>
<xml_diff>
--- a/Raw_data/location_data_full.xlsx
+++ b/Raw_data/location_data_full.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bop22abs/Documents/PhD/Chapter_1_code/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDFFBD1E-FADB-3342-AC41-10306BF64B18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED5BD384-EBCE-994E-A1A2-48A7BA775DEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" xr2:uid="{7DB4B7B0-8D04-9C4D-8F34-A11A49669C1B}"/>
   </bookViews>
@@ -8428,8 +8428,8 @@
   <dimension ref="A1:I777"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A335" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F344" sqref="F344"/>
+      <pane ySplit="1" topLeftCell="A438" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C451" sqref="C451"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>